<commit_message>
change the orderline status to be INVOICED when the invoice is generated
</commit_message>
<xml_diff>
--- a/results/Invoice/Invoice.xlsx
+++ b/results/Invoice/Invoice.xlsx
@@ -591,7 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -798,11 +798,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,7 +1172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
@@ -1320,60 +1321,28 @@
           <t>TO:</t>
         </is>
       </c>
-      <c r="B6" s="60" t="inlineStr">
-        <is>
-          <t>NORRISEAL-WELLMARK</t>
-        </is>
-      </c>
+      <c r="B6" s="60" t="inlineStr"/>
       <c r="M6" s="12" t="inlineStr">
         <is>
           <t>SHIP TO:</t>
         </is>
       </c>
-      <c r="N6" s="69" t="inlineStr">
-        <is>
-          <t>NORRISEAL-WELLMARK, INC</t>
-        </is>
-      </c>
+      <c r="N6" s="69" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="n"/>
-      <c r="B7" s="60" t="inlineStr">
-        <is>
-          <t>11122 WEST LITTLE YORK</t>
-        </is>
-      </c>
-      <c r="N7" s="69" t="inlineStr">
-        <is>
-          <t>11122 WEST LITTLE YORK</t>
-        </is>
-      </c>
+      <c r="B7" s="60" t="inlineStr"/>
+      <c r="N7" s="69" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n"/>
-      <c r="B8" s="60" t="inlineStr">
-        <is>
-          <t>HOUSTON, TX 77041</t>
-        </is>
-      </c>
-      <c r="N8" s="69" t="inlineStr">
-        <is>
-          <t>HOUSTON, TX 77041</t>
-        </is>
-      </c>
+      <c r="B8" s="60" t="inlineStr"/>
+      <c r="N8" s="69" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="n"/>
-      <c r="B9" s="60" t="inlineStr">
-        <is>
-          <t>U.S.A.</t>
-        </is>
-      </c>
-      <c r="N9" s="69" t="inlineStr">
-        <is>
-          <t>U.S.A.</t>
-        </is>
-      </c>
+      <c r="B9" s="60" t="inlineStr"/>
+      <c r="N9" s="69" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="n"/>
@@ -1625,7 +1594,7 @@
       <c r="C16" s="96" t="n"/>
       <c r="D16" s="95" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E16" s="95" t="inlineStr">
@@ -1641,7 +1610,7 @@
       </c>
       <c r="H16" s="96" t="n"/>
       <c r="I16" s="95" t="n">
-        <v>4900</v>
+        <v>5000</v>
       </c>
       <c r="J16" s="95" t="n"/>
       <c r="K16" s="95" t="n"/>
@@ -1658,9 +1627,7 @@
           <t>0%</t>
         </is>
       </c>
-      <c r="O16" s="95" t="n">
-        <v>10</v>
-      </c>
+      <c r="O16" s="95" t="n"/>
       <c r="P16" s="95" t="n">
         <v>0</v>
       </c>
@@ -1668,7 +1635,7 @@
         <v>3.8</v>
       </c>
       <c r="R16" s="95" t="n">
-        <v>18620</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="17" ht="14" customHeight="1" thickTop="1">
@@ -1683,7 +1650,7 @@
       <c r="C17" s="96" t="n"/>
       <c r="D17" s="95" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E17" s="95" t="inlineStr">
@@ -1728,186 +1695,130 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="95" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="95" t="inlineStr">
-        <is>
-          <t>bbbb</t>
-        </is>
-      </c>
-      <c r="C18" s="96" t="n"/>
-      <c r="D18" s="95" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E18" s="95" t="inlineStr">
-        <is>
-          <t>01008-1404</t>
-        </is>
-      </c>
-      <c r="F18" s="96" t="n"/>
-      <c r="G18" s="95" t="inlineStr">
-        <is>
-          <t>SADDLE</t>
-        </is>
-      </c>
-      <c r="H18" s="96" t="n"/>
-      <c r="I18" s="95" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J18" s="95" t="n"/>
-      <c r="K18" s="95" t="n"/>
-      <c r="L18" s="95" t="inlineStr">
-        <is>
-          <t>DI</t>
-        </is>
-      </c>
-      <c r="M18" s="95" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="N18" s="95" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O18" s="95" t="n"/>
-      <c r="P18" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="95" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="R18" s="95" t="n">
-        <v>19000</v>
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   MAKE ALL CHECKS PAYABLE TO ITE, INC.</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n"/>
+      <c r="C18" s="7" t="n"/>
+      <c r="D18" s="7" t="n"/>
+      <c r="E18" s="24" t="n"/>
+      <c r="F18" s="7" t="n"/>
+      <c r="G18" s="7" t="n"/>
+      <c r="H18" s="7" t="n"/>
+      <c r="I18" s="7" t="n"/>
+      <c r="J18" s="7" t="n"/>
+      <c r="K18" s="84" t="n"/>
+      <c r="L18" s="84" t="n"/>
+      <c r="M18" s="84" t="n"/>
+      <c r="N18" s="14" t="n"/>
+      <c r="O18" s="84" t="n"/>
+      <c r="P18" s="84" t="inlineStr">
+        <is>
+          <t>TOTAL DUE(USD):</t>
+        </is>
+      </c>
+      <c r="Q18" s="85" t="n"/>
+      <c r="R18" s="97" t="n">
+        <v>38000</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   MAKE ALL CHECKS PAYABLE TO ITE, INC.</t>
-        </is>
-      </c>
-      <c r="B19" s="7" t="n"/>
-      <c r="C19" s="7" t="n"/>
-      <c r="D19" s="7" t="n"/>
-      <c r="E19" s="24" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="7" t="n"/>
-      <c r="I19" s="7" t="n"/>
-      <c r="J19" s="7" t="n"/>
-      <c r="K19" s="84" t="n"/>
-      <c r="L19" s="84" t="n"/>
-      <c r="M19" s="84" t="n"/>
-      <c r="N19" s="14" t="n"/>
-      <c r="O19" s="84" t="n"/>
-      <c r="P19" s="84" t="inlineStr">
-        <is>
-          <t>TOTAL DUE(USD):</t>
-        </is>
-      </c>
-      <c r="Q19" s="85" t="n"/>
-      <c r="R19" s="97" t="n">
-        <v>56620</v>
-      </c>
+      <c r="A19" s="98" t="inlineStr">
+        <is>
+          <t>ITE USE ONLY</t>
+        </is>
+      </c>
+      <c r="B19" s="99" t="n"/>
+      <c r="C19" s="99" t="n"/>
+      <c r="D19" s="99" t="n"/>
+      <c r="E19" s="99" t="n"/>
+      <c r="F19" s="99" t="n"/>
+      <c r="G19" s="99" t="n"/>
+      <c r="H19" s="99" t="n"/>
+      <c r="I19" s="99" t="n"/>
+      <c r="J19" s="100" t="n"/>
+      <c r="K19" s="50" t="inlineStr">
+        <is>
+          <t>MANUFACTURED BY:</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="n"/>
     </row>
     <row r="20" ht="14" customHeight="1" thickBot="1">
-      <c r="A20" s="98" t="inlineStr">
-        <is>
-          <t>ITE USE ONLY</t>
-        </is>
-      </c>
-      <c r="B20" s="99" t="n"/>
-      <c r="C20" s="99" t="n"/>
-      <c r="D20" s="99" t="n"/>
-      <c r="E20" s="99" t="n"/>
-      <c r="F20" s="99" t="n"/>
-      <c r="G20" s="99" t="n"/>
-      <c r="H20" s="99" t="n"/>
-      <c r="I20" s="99" t="n"/>
-      <c r="J20" s="100" t="n"/>
-      <c r="K20" s="50" t="inlineStr">
-        <is>
-          <t>MANUFACTURED BY:</t>
+      <c r="A20" s="101" t="inlineStr">
+        <is>
+          <t>fcrq</t>
+        </is>
+      </c>
+      <c r="B20" s="47" t="n"/>
+      <c r="C20" s="45" t="inlineStr">
+        <is>
+          <t>cwdz</t>
+        </is>
+      </c>
+      <c r="D20" s="47" t="n"/>
+      <c r="E20" s="33" t="inlineStr">
+        <is>
+          <t>zffs</t>
+        </is>
+      </c>
+      <c r="F20" s="34" t="inlineStr">
+        <is>
+          <t>zfrq</t>
+        </is>
+      </c>
+      <c r="G20" s="34" t="inlineStr">
+        <is>
+          <t>crzh</t>
+        </is>
+      </c>
+      <c r="H20" s="34" t="inlineStr">
+        <is>
+          <t>crje</t>
+        </is>
+      </c>
+      <c r="I20" s="34" t="inlineStr">
+        <is>
+          <t>fkbl</t>
+        </is>
+      </c>
+      <c r="J20" s="28" t="inlineStr">
+        <is>
+          <t>tgi</t>
         </is>
       </c>
       <c r="N20" s="3" t="n"/>
     </row>
     <row r="21" ht="14" customHeight="1" thickTop="1">
-      <c r="A21" s="46" t="inlineStr">
-        <is>
-          <t>fcrq</t>
-        </is>
-      </c>
-      <c r="B21" s="47" t="n"/>
-      <c r="C21" s="45" t="inlineStr">
-        <is>
-          <t>cwdz</t>
-        </is>
-      </c>
-      <c r="D21" s="47" t="n"/>
-      <c r="E21" s="33" t="inlineStr">
-        <is>
-          <t>zffs</t>
-        </is>
-      </c>
-      <c r="F21" s="34" t="inlineStr">
-        <is>
-          <t>zfrq</t>
-        </is>
-      </c>
-      <c r="G21" s="34" t="inlineStr">
-        <is>
-          <t>crzh</t>
-        </is>
-      </c>
-      <c r="H21" s="34" t="inlineStr">
-        <is>
-          <t>crje</t>
-        </is>
-      </c>
-      <c r="I21" s="34" t="inlineStr">
-        <is>
-          <t>fkbl</t>
-        </is>
-      </c>
-      <c r="J21" s="28" t="inlineStr">
-        <is>
-          <t>tgi</t>
-        </is>
-      </c>
+      <c r="A21" s="48" t="n"/>
+      <c r="B21" s="49" t="n"/>
+      <c r="C21" s="54" t="n"/>
+      <c r="D21" s="55" t="n"/>
+      <c r="E21" s="36" t="n"/>
+      <c r="F21" s="37" t="n"/>
+      <c r="G21" s="37" t="n"/>
+      <c r="H21" s="37" t="n"/>
+      <c r="I21" s="37" t="n"/>
+      <c r="J21" s="38" t="n"/>
       <c r="N21" s="3" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="48" t="n"/>
-      <c r="B22" s="49" t="n"/>
-      <c r="C22" s="54" t="n"/>
-      <c r="D22" s="55" t="n"/>
-      <c r="E22" s="36" t="n"/>
-      <c r="F22" s="37" t="n"/>
-      <c r="G22" s="37" t="n"/>
-      <c r="H22" s="37" t="n"/>
-      <c r="I22" s="37" t="n"/>
-      <c r="J22" s="38" t="n"/>
+      <c r="A22" s="42" t="n"/>
+      <c r="B22" s="43" t="n"/>
+      <c r="C22" s="44" t="n"/>
+      <c r="D22" s="43" t="n"/>
+      <c r="E22" s="40" t="n"/>
+      <c r="F22" s="39" t="n"/>
+      <c r="G22" s="39" t="n"/>
+      <c r="H22" s="39" t="n"/>
+      <c r="I22" s="39" t="n"/>
+      <c r="J22" s="41" t="n"/>
       <c r="N22" s="3" t="n"/>
     </row>
-    <row r="23">
-      <c r="A23" s="42" t="n"/>
-      <c r="B23" s="43" t="n"/>
-      <c r="C23" s="44" t="n"/>
-      <c r="D23" s="43" t="n"/>
-      <c r="E23" s="40" t="n"/>
-      <c r="F23" s="39" t="n"/>
-      <c r="G23" s="39" t="n"/>
-      <c r="H23" s="39" t="n"/>
-      <c r="I23" s="39" t="n"/>
-      <c r="J23" s="41" t="n"/>
-      <c r="N23" s="3" t="n"/>
-    </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="44">
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="Q3:R3"/>
@@ -1915,12 +1826,11 @@
     <mergeCell ref="N7:R7"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="B8:G8"/>
-    <mergeCell ref="A20:J20"/>
     <mergeCell ref="G14:H15"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:C18"/>
     <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A19:J19"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="K11:L11"/>
@@ -1928,7 +1838,6 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="N8:R8"/>
@@ -1954,7 +1863,6 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="N6:R6"/>
     <mergeCell ref="B14:C15"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" scale="72" horizontalDpi="4294967292" verticalDpi="300"/>

</xml_diff>

<commit_message>
add extra charges to the invoice
</commit_message>
<xml_diff>
--- a/results/Invoice/Invoice.xlsx
+++ b/results/Invoice/Invoice.xlsx
@@ -1461,11 +1461,7 @@
       <c r="A12" s="61" t="n"/>
       <c r="B12" s="87" t="n"/>
       <c r="C12" s="88" t="n"/>
-      <c r="D12" s="60" t="inlineStr">
-        <is>
-          <t>Sea</t>
-        </is>
-      </c>
+      <c r="D12" s="60" t="n"/>
       <c r="E12" s="88" t="n"/>
       <c r="F12" s="60" t="inlineStr">
         <is>
@@ -1474,7 +1470,7 @@
       </c>
       <c r="G12" s="88" t="n"/>
       <c r="H12" s="60" t="n"/>
-      <c r="I12" s="60" t="inlineStr"/>
+      <c r="I12" s="60" t="n"/>
       <c r="J12" s="88" t="n"/>
       <c r="K12" s="60" t="n"/>
       <c r="L12" s="88" t="n"/>
@@ -1629,120 +1625,64 @@
       <c r="A16" s="95" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="95" t="inlineStr">
-        <is>
-          <t>bbbb</t>
-        </is>
-      </c>
+      <c r="B16" s="95" t="n"/>
       <c r="C16" s="96" t="n"/>
-      <c r="D16" s="95" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E16" s="95" t="inlineStr">
-        <is>
-          <t>01008-1404</t>
-        </is>
-      </c>
+      <c r="D16" s="95" t="n"/>
+      <c r="E16" s="95" t="n"/>
       <c r="F16" s="96" t="n"/>
       <c r="G16" s="95" t="inlineStr">
         <is>
-          <t>SADDLE</t>
+          <t>test</t>
         </is>
       </c>
       <c r="H16" s="96" t="n"/>
       <c r="I16" s="95" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J16" s="95" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J16" s="95" t="n"/>
       <c r="K16" s="95" t="n"/>
-      <c r="L16" s="95" t="inlineStr">
-        <is>
-          <t>DI</t>
-        </is>
-      </c>
-      <c r="M16" s="95" t="n">
-        <v>3.23</v>
-      </c>
-      <c r="N16" s="95" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
+      <c r="L16" s="95" t="n"/>
+      <c r="M16" s="95" t="n"/>
+      <c r="N16" s="95" t="n"/>
       <c r="O16" s="95" t="n"/>
-      <c r="P16" s="95" t="n">
-        <v>0</v>
-      </c>
+      <c r="P16" s="95" t="n"/>
       <c r="Q16" s="95" t="n">
-        <v>3.23</v>
+        <v>10</v>
       </c>
       <c r="R16" s="95" t="n">
-        <v>16150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" ht="14" customHeight="1" thickTop="1">
       <c r="A17" s="95" t="n">
         <v>2</v>
       </c>
-      <c r="B17" s="95" t="inlineStr">
-        <is>
-          <t>bbbb</t>
-        </is>
-      </c>
+      <c r="B17" s="95" t="n"/>
       <c r="C17" s="96" t="n"/>
-      <c r="D17" s="95" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E17" s="95" t="inlineStr">
-        <is>
-          <t>01008-1404</t>
-        </is>
-      </c>
+      <c r="D17" s="95" t="n"/>
+      <c r="E17" s="95" t="n"/>
       <c r="F17" s="96" t="n"/>
       <c r="G17" s="95" t="inlineStr">
         <is>
-          <t>Surcharge test</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="H17" s="96" t="n"/>
       <c r="I17" s="95" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J17" s="95" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J17" s="95" t="n"/>
       <c r="K17" s="95" t="n"/>
-      <c r="L17" s="95" t="inlineStr">
-        <is>
-          <t>DI</t>
-        </is>
-      </c>
-      <c r="M17" s="95" t="n">
-        <v>3.23</v>
-      </c>
-      <c r="N17" s="95" t="inlineStr">
-        <is>
-          <t>10.0%</t>
-        </is>
-      </c>
+      <c r="L17" s="95" t="n"/>
+      <c r="M17" s="95" t="n"/>
+      <c r="N17" s="95" t="n"/>
       <c r="O17" s="95" t="n"/>
-      <c r="P17" s="95" t="n">
-        <v>0.32</v>
-      </c>
+      <c r="P17" s="95" t="n"/>
       <c r="Q17" s="95" t="n">
-        <v>0.32</v>
+        <v>15</v>
       </c>
       <c r="R17" s="95" t="n">
-        <v>1600</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
@@ -1772,7 +1712,7 @@
       </c>
       <c r="Q18" s="56" t="n"/>
       <c r="R18" s="97" t="n">
-        <v>17750</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
change the style of the ship via block
</commit_message>
<xml_diff>
--- a/results/Invoice/Invoice.xlsx
+++ b/results/Invoice/Invoice.xlsx
@@ -1219,7 +1219,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
@@ -1461,7 +1461,11 @@
       <c r="A12" s="61" t="n"/>
       <c r="B12" s="87" t="n"/>
       <c r="C12" s="88" t="n"/>
-      <c r="D12" s="60" t="n"/>
+      <c r="D12" s="60" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
       <c r="E12" s="88" t="n"/>
       <c r="F12" s="60" t="inlineStr">
         <is>
@@ -1470,7 +1474,7 @@
       </c>
       <c r="G12" s="88" t="n"/>
       <c r="H12" s="60" t="n"/>
-      <c r="I12" s="60" t="n"/>
+      <c r="I12" s="60" t="inlineStr"/>
       <c r="J12" s="88" t="n"/>
       <c r="K12" s="60" t="n"/>
       <c r="L12" s="88" t="n"/>
@@ -1625,191 +1629,187 @@
       <c r="A16" s="95" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="95" t="n"/>
+      <c r="B16" s="95" t="inlineStr">
+        <is>
+          <t>bbbb</t>
+        </is>
+      </c>
       <c r="C16" s="96" t="n"/>
-      <c r="D16" s="95" t="n"/>
-      <c r="E16" s="95" t="n"/>
+      <c r="D16" s="95" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E16" s="95" t="inlineStr">
+        <is>
+          <t>01008-1404</t>
+        </is>
+      </c>
       <c r="F16" s="96" t="n"/>
       <c r="G16" s="95" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>SADDLE</t>
         </is>
       </c>
       <c r="H16" s="96" t="n"/>
       <c r="I16" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="J16" s="95" t="n"/>
+        <v>5000</v>
+      </c>
+      <c r="J16" s="95" t="inlineStr">
+        <is>
+          <t>EACH</t>
+        </is>
+      </c>
       <c r="K16" s="95" t="n"/>
-      <c r="L16" s="95" t="n"/>
-      <c r="M16" s="95" t="n"/>
-      <c r="N16" s="95" t="n"/>
+      <c r="L16" s="95" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="M16" s="95" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="N16" s="95" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="O16" s="95" t="n"/>
-      <c r="P16" s="95" t="n"/>
+      <c r="P16" s="95" t="n">
+        <v>0</v>
+      </c>
       <c r="Q16" s="95" t="n">
-        <v>10</v>
+        <v>3.8</v>
       </c>
       <c r="R16" s="95" t="n">
-        <v>20</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="17" ht="14" customHeight="1" thickTop="1">
-      <c r="A17" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="95" t="n"/>
-      <c r="C17" s="96" t="n"/>
-      <c r="D17" s="95" t="n"/>
-      <c r="E17" s="95" t="n"/>
-      <c r="F17" s="96" t="n"/>
-      <c r="G17" s="95" t="inlineStr">
-        <is>
-          <t>test2</t>
-        </is>
-      </c>
-      <c r="H17" s="96" t="n"/>
-      <c r="I17" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="J17" s="95" t="n"/>
-      <c r="K17" s="95" t="n"/>
-      <c r="L17" s="95" t="n"/>
-      <c r="M17" s="95" t="n"/>
-      <c r="N17" s="95" t="n"/>
-      <c r="O17" s="95" t="n"/>
-      <c r="P17" s="95" t="n"/>
-      <c r="Q17" s="95" t="n">
-        <v>15</v>
-      </c>
-      <c r="R17" s="95" t="n">
-        <v>30</v>
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   MAKE ALL CHECKS PAYABLE TO ITE, INC.</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n"/>
+      <c r="C17" s="7" t="n"/>
+      <c r="D17" s="7" t="n"/>
+      <c r="E17" s="24" t="n"/>
+      <c r="F17" s="7" t="n"/>
+      <c r="G17" s="7" t="n"/>
+      <c r="H17" s="7" t="n"/>
+      <c r="I17" s="7" t="n"/>
+      <c r="J17" s="7" t="n"/>
+      <c r="K17" s="13" t="n"/>
+      <c r="L17" s="13" t="n"/>
+      <c r="M17" s="13" t="n"/>
+      <c r="N17" s="14" t="n"/>
+      <c r="O17" s="13" t="n"/>
+      <c r="P17" s="13" t="inlineStr">
+        <is>
+          <t>TOTAL DUE(USD):</t>
+        </is>
+      </c>
+      <c r="Q17" s="56" t="n"/>
+      <c r="R17" s="97" t="n">
+        <v>19000</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   MAKE ALL CHECKS PAYABLE TO ITE, INC.</t>
-        </is>
-      </c>
-      <c r="B18" s="7" t="n"/>
-      <c r="C18" s="7" t="n"/>
-      <c r="D18" s="7" t="n"/>
-      <c r="E18" s="24" t="n"/>
-      <c r="F18" s="7" t="n"/>
-      <c r="G18" s="7" t="n"/>
-      <c r="H18" s="7" t="n"/>
-      <c r="I18" s="7" t="n"/>
-      <c r="J18" s="7" t="n"/>
-      <c r="K18" s="13" t="n"/>
-      <c r="L18" s="13" t="n"/>
-      <c r="M18" s="13" t="n"/>
-      <c r="N18" s="14" t="n"/>
-      <c r="O18" s="13" t="n"/>
-      <c r="P18" s="13" t="inlineStr">
-        <is>
-          <t>TOTAL DUE(USD):</t>
-        </is>
-      </c>
-      <c r="Q18" s="56" t="n"/>
-      <c r="R18" s="97" t="n">
-        <v>50</v>
-      </c>
+      <c r="A18" s="98" t="inlineStr">
+        <is>
+          <t>ITE USE ONLY</t>
+        </is>
+      </c>
+      <c r="B18" s="99" t="n"/>
+      <c r="C18" s="99" t="n"/>
+      <c r="D18" s="99" t="n"/>
+      <c r="E18" s="99" t="n"/>
+      <c r="F18" s="99" t="n"/>
+      <c r="G18" s="99" t="n"/>
+      <c r="H18" s="99" t="n"/>
+      <c r="I18" s="99" t="n"/>
+      <c r="J18" s="100" t="n"/>
+      <c r="K18" s="50" t="inlineStr">
+        <is>
+          <t>MANUFACTURED BY:</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="98" t="inlineStr">
-        <is>
-          <t>ITE USE ONLY</t>
-        </is>
-      </c>
-      <c r="B19" s="99" t="n"/>
-      <c r="C19" s="99" t="n"/>
-      <c r="D19" s="99" t="n"/>
-      <c r="E19" s="99" t="n"/>
-      <c r="F19" s="99" t="n"/>
-      <c r="G19" s="99" t="n"/>
-      <c r="H19" s="99" t="n"/>
-      <c r="I19" s="99" t="n"/>
-      <c r="J19" s="100" t="n"/>
-      <c r="K19" s="50" t="inlineStr">
-        <is>
-          <t>MANUFACTURED BY:</t>
+      <c r="A19" s="46" t="inlineStr">
+        <is>
+          <t>fcrq</t>
+        </is>
+      </c>
+      <c r="B19" s="47" t="n"/>
+      <c r="C19" s="45" t="inlineStr">
+        <is>
+          <t>cwdz</t>
+        </is>
+      </c>
+      <c r="D19" s="47" t="n"/>
+      <c r="E19" s="33" t="inlineStr">
+        <is>
+          <t>zffs</t>
+        </is>
+      </c>
+      <c r="F19" s="34" t="inlineStr">
+        <is>
+          <t>zfrq</t>
+        </is>
+      </c>
+      <c r="G19" s="34" t="inlineStr">
+        <is>
+          <t>crzh</t>
+        </is>
+      </c>
+      <c r="H19" s="34" t="inlineStr">
+        <is>
+          <t>crje</t>
+        </is>
+      </c>
+      <c r="I19" s="34" t="inlineStr">
+        <is>
+          <t>fkbl</t>
+        </is>
+      </c>
+      <c r="J19" s="28" t="inlineStr">
+        <is>
+          <t>tgi</t>
         </is>
       </c>
       <c r="N19" s="3" t="n"/>
     </row>
     <row r="20" ht="14" customHeight="1" thickBot="1">
-      <c r="A20" s="46" t="inlineStr">
-        <is>
-          <t>fcrq</t>
-        </is>
-      </c>
-      <c r="B20" s="47" t="n"/>
-      <c r="C20" s="45" t="inlineStr">
-        <is>
-          <t>cwdz</t>
-        </is>
-      </c>
-      <c r="D20" s="47" t="n"/>
-      <c r="E20" s="33" t="inlineStr">
-        <is>
-          <t>zffs</t>
-        </is>
-      </c>
-      <c r="F20" s="34" t="inlineStr">
-        <is>
-          <t>zfrq</t>
-        </is>
-      </c>
-      <c r="G20" s="34" t="inlineStr">
-        <is>
-          <t>crzh</t>
-        </is>
-      </c>
-      <c r="H20" s="34" t="inlineStr">
-        <is>
-          <t>crje</t>
-        </is>
-      </c>
-      <c r="I20" s="34" t="inlineStr">
-        <is>
-          <t>fkbl</t>
-        </is>
-      </c>
-      <c r="J20" s="28" t="inlineStr">
-        <is>
-          <t>tgi</t>
-        </is>
-      </c>
+      <c r="A20" s="48" t="n"/>
+      <c r="B20" s="49" t="n"/>
+      <c r="C20" s="54" t="n"/>
+      <c r="D20" s="55" t="n"/>
+      <c r="E20" s="36" t="n"/>
+      <c r="F20" s="37" t="n"/>
+      <c r="G20" s="37" t="n"/>
+      <c r="H20" s="37" t="n"/>
+      <c r="I20" s="37" t="n"/>
+      <c r="J20" s="38" t="n"/>
       <c r="N20" s="3" t="n"/>
     </row>
     <row r="21" ht="14" customHeight="1" thickTop="1">
-      <c r="A21" s="48" t="n"/>
-      <c r="B21" s="49" t="n"/>
-      <c r="C21" s="54" t="n"/>
-      <c r="D21" s="55" t="n"/>
-      <c r="E21" s="36" t="n"/>
-      <c r="F21" s="37" t="n"/>
-      <c r="G21" s="37" t="n"/>
-      <c r="H21" s="37" t="n"/>
-      <c r="I21" s="37" t="n"/>
-      <c r="J21" s="38" t="n"/>
+      <c r="A21" s="42" t="n"/>
+      <c r="B21" s="43" t="n"/>
+      <c r="C21" s="44" t="n"/>
+      <c r="D21" s="43" t="n"/>
+      <c r="E21" s="40" t="n"/>
+      <c r="F21" s="39" t="n"/>
+      <c r="G21" s="39" t="n"/>
+      <c r="H21" s="39" t="n"/>
+      <c r="I21" s="39" t="n"/>
+      <c r="J21" s="41" t="n"/>
       <c r="N21" s="3" t="n"/>
     </row>
-    <row r="22">
-      <c r="A22" s="42" t="n"/>
-      <c r="B22" s="43" t="n"/>
-      <c r="C22" s="44" t="n"/>
-      <c r="D22" s="43" t="n"/>
-      <c r="E22" s="40" t="n"/>
-      <c r="F22" s="39" t="n"/>
-      <c r="G22" s="39" t="n"/>
-      <c r="H22" s="39" t="n"/>
-      <c r="I22" s="39" t="n"/>
-      <c r="J22" s="41" t="n"/>
-      <c r="N22" s="3" t="n"/>
-    </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="42">
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="Q3:R3"/>
@@ -1820,16 +1820,12 @@
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="G14:H15"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="A19:J19"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="N8:R8"/>
@@ -1853,6 +1849,7 @@
     <mergeCell ref="Q11:R11"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A18:J18"/>
     <mergeCell ref="N6:R6"/>
     <mergeCell ref="B14:C15"/>
   </mergeCells>

</xml_diff>